<commit_message>
updated as of 30th April 2025: README updated to match the charts.docx file contents. Dates, Hours and Value for Money all updated in XLSX files.
</commit_message>
<xml_diff>
--- a/playstation/output/1. wishlist.xlsx
+++ b/playstation/output/1. wishlist.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="2025-03-31" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="2025-04-30" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="wishlist" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
@@ -495,6 +495,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FF00FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
@@ -509,18 +521,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF00FFFF"/>
         <bgColor rgb="FF00FFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00FF00"/>
-        <bgColor rgb="FF00FF00"/>
       </patternFill>
     </fill>
     <fill>
@@ -580,7 +580,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -611,52 +611,61 @@
     <xf borderId="1" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
+    <xf borderId="1" fillId="6" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="1" fillId="3" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="7" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="5" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="7" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
+    <xf borderId="1" fillId="7" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="7" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="7" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="7" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="7" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
     <xf borderId="1" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -674,7 +683,7 @@
     <xf borderId="2" fillId="0" fontId="4" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="3" fillId="6" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="4" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -692,13 +701,7 @@
     <xf borderId="4" fillId="0" fontId="4" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="7" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="9" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="9" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -707,10 +710,10 @@
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="8" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="8" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="5" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1092,13 +1095,13 @@
       <c r="A3" s="4">
         <v>1084.0</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="10" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="11">
         <v>45490.0</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -1110,22 +1113,22 @@
       <c r="G3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="11">
+      <c r="H3" s="12">
         <v>19.99</v>
       </c>
-      <c r="I3" s="11">
-        <v>19.99</v>
-      </c>
-      <c r="J3" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="I3" s="12">
+        <v>13.99</v>
+      </c>
+      <c r="J3" s="13">
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="K3" s="8">
         <v>1.0</v>
       </c>
       <c r="L3" s="9">
         <f t="shared" si="2"/>
-        <v>19.99</v>
+        <v>13.99</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>22</v>
@@ -1144,7 +1147,7 @@
       <c r="C4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="14">
         <v>45923.0</v>
       </c>
       <c r="E4" s="5" t="s">
@@ -1236,7 +1239,7 @@
       <c r="C6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="11">
         <v>35699.0</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -1248,11 +1251,11 @@
       <c r="G6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="11">
-        <v>19.99</v>
-      </c>
-      <c r="I6" s="11">
-        <v>19.99</v>
+      <c r="H6" s="12">
+        <v>29.99</v>
+      </c>
+      <c r="I6" s="12">
+        <v>29.99</v>
       </c>
       <c r="J6" s="7">
         <f t="shared" si="1"/>
@@ -1263,7 +1266,7 @@
       </c>
       <c r="L6" s="9">
         <f t="shared" si="2"/>
-        <v>19.99</v>
+        <v>29.99</v>
       </c>
       <c r="M6" s="4" t="s">
         <v>31</v>
@@ -1282,7 +1285,7 @@
       <c r="C7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="11">
         <v>44154.0</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -1294,10 +1297,10 @@
       <c r="G7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="12">
         <v>79.99</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="12">
         <v>79.99</v>
       </c>
       <c r="J7" s="7">
@@ -1322,45 +1325,45 @@
       <c r="A8" s="4">
         <v>1089.0</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="14">
+      <c r="D8" s="16">
         <v>36462.0</v>
       </c>
-      <c r="E8" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="15">
+      <c r="E8" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="17">
         <v>9.99</v>
       </c>
-      <c r="I8" s="15">
+      <c r="I8" s="17">
         <v>9.99</v>
       </c>
       <c r="J8" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K8" s="16">
-        <v>1.0</v>
-      </c>
-      <c r="L8" s="17">
+      <c r="K8" s="18">
+        <v>1.0</v>
+      </c>
+      <c r="L8" s="19">
         <f t="shared" si="2"/>
         <v>9.99</v>
       </c>
-      <c r="M8" s="13" t="s">
+      <c r="M8" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="N8" s="13" t="s">
+      <c r="N8" s="15" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1368,45 +1371,45 @@
       <c r="A9" s="4">
         <v>1090.0</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="16">
         <v>36854.0</v>
       </c>
-      <c r="E9" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="15">
+      <c r="E9" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="17">
         <v>9.99</v>
       </c>
-      <c r="I9" s="15">
+      <c r="I9" s="17">
         <v>9.99</v>
       </c>
       <c r="J9" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K9" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="L9" s="19">
+      <c r="K9" s="20">
+        <v>1.0</v>
+      </c>
+      <c r="L9" s="21">
         <f t="shared" si="2"/>
         <v>9.99</v>
       </c>
-      <c r="M9" s="20" t="s">
+      <c r="M9" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="N9" s="20" t="s">
+      <c r="N9" s="22" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1414,45 +1417,45 @@
       <c r="A10" s="4">
         <v>1091.0</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="16">
         <v>35727.0</v>
       </c>
-      <c r="E10" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="15">
+      <c r="E10" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="17">
         <v>9.99</v>
       </c>
-      <c r="I10" s="15">
+      <c r="I10" s="17">
         <v>9.99</v>
       </c>
       <c r="J10" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K10" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="L10" s="19">
+      <c r="K10" s="20">
+        <v>1.0</v>
+      </c>
+      <c r="L10" s="21">
         <f t="shared" si="2"/>
         <v>9.99</v>
       </c>
-      <c r="M10" s="20" t="s">
+      <c r="M10" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="N10" s="20" t="s">
+      <c r="N10" s="22" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1696,39 +1699,39 @@
       <c r="C16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="11">
         <v>45735.0</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F16" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="21">
+      <c r="F16" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="23">
         <v>21.99</v>
       </c>
-      <c r="I16" s="21">
+      <c r="I16" s="23">
         <v>21.99</v>
       </c>
       <c r="J16" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K16" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="L16" s="19">
+      <c r="K16" s="20">
+        <v>1.0</v>
+      </c>
+      <c r="L16" s="21">
         <f t="shared" si="2"/>
         <v>21.99</v>
       </c>
-      <c r="M16" s="20" t="s">
+      <c r="M16" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="N16" s="20" t="s">
+      <c r="N16" s="22" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1739,42 +1742,42 @@
       <c r="B17" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="22">
+      <c r="D17" s="24">
         <v>36406.0</v>
       </c>
-      <c r="E17" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" s="21">
+      <c r="E17" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="23">
         <v>15.0</v>
       </c>
-      <c r="I17" s="21">
+      <c r="I17" s="23">
         <v>15.0</v>
       </c>
       <c r="J17" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K17" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="L17" s="19">
+      <c r="K17" s="20">
+        <v>1.0</v>
+      </c>
+      <c r="L17" s="21">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="M17" s="20" t="s">
+      <c r="M17" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="N17" s="20" t="s">
+      <c r="N17" s="22" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1785,42 +1788,42 @@
       <c r="B18" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="22">
+      <c r="D18" s="24">
         <v>37218.0</v>
       </c>
-      <c r="E18" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="G18" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="H18" s="21">
+      <c r="E18" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H18" s="23">
         <v>14.99</v>
       </c>
-      <c r="I18" s="21">
+      <c r="I18" s="23">
         <v>14.99</v>
       </c>
       <c r="J18" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K18" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="L18" s="19">
+      <c r="K18" s="20">
+        <v>1.0</v>
+      </c>
+      <c r="L18" s="21">
         <f t="shared" si="2"/>
         <v>14.99</v>
       </c>
-      <c r="M18" s="20" t="s">
+      <c r="M18" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="N18" s="20" t="s">
+      <c r="N18" s="22" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1828,45 +1831,45 @@
       <c r="A19" s="4">
         <v>1100.0</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D19" s="16">
         <v>45125.0</v>
       </c>
-      <c r="E19" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="H19" s="15">
+      <c r="E19" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19" s="17">
         <v>12.5</v>
       </c>
-      <c r="I19" s="15">
-        <v>12.5</v>
-      </c>
-      <c r="J19" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K19" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="L19" s="19">
-        <f t="shared" si="2"/>
-        <v>12.5</v>
-      </c>
-      <c r="M19" s="20" t="s">
+      <c r="I19" s="17">
+        <v>8.12</v>
+      </c>
+      <c r="J19" s="13">
+        <f t="shared" si="1"/>
+        <v>4.38</v>
+      </c>
+      <c r="K19" s="20">
+        <v>1.0</v>
+      </c>
+      <c r="L19" s="21">
+        <f t="shared" si="2"/>
+        <v>8.12</v>
+      </c>
+      <c r="M19" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="N19" s="20" t="s">
+      <c r="N19" s="22" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1874,45 +1877,45 @@
       <c r="A20" s="4">
         <v>1101.0</v>
       </c>
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="16">
         <v>45125.0</v>
       </c>
-      <c r="E20" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="H20" s="15">
+      <c r="E20" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20" s="17">
         <v>12.49</v>
       </c>
-      <c r="I20" s="15">
-        <v>12.49</v>
-      </c>
-      <c r="J20" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K20" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="L20" s="19">
-        <f t="shared" si="2"/>
-        <v>12.49</v>
-      </c>
-      <c r="M20" s="20" t="s">
+      <c r="I20" s="17">
+        <v>8.12</v>
+      </c>
+      <c r="J20" s="13">
+        <f t="shared" si="1"/>
+        <v>4.37</v>
+      </c>
+      <c r="K20" s="20">
+        <v>1.0</v>
+      </c>
+      <c r="L20" s="21">
+        <f t="shared" si="2"/>
+        <v>8.12</v>
+      </c>
+      <c r="M20" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="N20" s="20" t="s">
+      <c r="N20" s="22" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1972,7 +1975,7 @@
       <c r="C22" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="11">
         <v>36637.0</v>
       </c>
       <c r="E22" s="4" t="s">
@@ -1984,10 +1987,10 @@
       <c r="G22" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H22" s="11">
+      <c r="H22" s="12">
         <v>9.99</v>
       </c>
-      <c r="I22" s="11">
+      <c r="I22" s="12">
         <v>9.99</v>
       </c>
       <c r="J22" s="7">
@@ -2012,13 +2015,13 @@
       <c r="A23" s="4">
         <v>1104.0</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="10" t="s">
         <v>68</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D23" s="11">
         <v>45611.0</v>
       </c>
       <c r="E23" s="4" t="s">
@@ -2030,27 +2033,27 @@
       <c r="G23" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H23" s="11">
+      <c r="H23" s="12">
         <v>17.99</v>
       </c>
-      <c r="I23" s="11">
-        <v>17.99</v>
-      </c>
-      <c r="J23" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="I23" s="12">
+        <v>14.39</v>
+      </c>
+      <c r="J23" s="13">
+        <f t="shared" si="1"/>
+        <v>3.6</v>
       </c>
       <c r="K23" s="8">
         <v>1.0</v>
       </c>
       <c r="L23" s="9">
         <f t="shared" si="2"/>
-        <v>17.99</v>
-      </c>
-      <c r="M23" s="24" t="s">
+        <v>14.39</v>
+      </c>
+      <c r="M23" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="N23" s="24" t="s">
+      <c r="N23" s="26" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2058,13 +2061,13 @@
       <c r="A24" s="4">
         <v>1105.0</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="10" t="s">
         <v>71</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="11">
         <v>45611.0</v>
       </c>
       <c r="E24" s="4" t="s">
@@ -2076,27 +2079,27 @@
       <c r="G24" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H24" s="11">
+      <c r="H24" s="12">
         <v>19.99</v>
       </c>
-      <c r="I24" s="11">
-        <v>19.99</v>
-      </c>
-      <c r="J24" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="I24" s="12">
+        <v>15.99</v>
+      </c>
+      <c r="J24" s="13">
+        <f t="shared" si="1"/>
+        <v>4</v>
       </c>
       <c r="K24" s="8">
         <v>1.0</v>
       </c>
       <c r="L24" s="9">
         <f t="shared" si="2"/>
-        <v>19.99</v>
-      </c>
-      <c r="M24" s="24" t="s">
+        <v>15.99</v>
+      </c>
+      <c r="M24" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="N24" s="24" t="s">
+      <c r="N24" s="26" t="s">
         <v>70</v>
       </c>
     </row>
@@ -2104,45 +2107,45 @@
       <c r="A25" s="4">
         <v>1106.0</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="14">
+      <c r="D25" s="16">
         <v>39500.0</v>
       </c>
-      <c r="E25" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F25" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="H25" s="15">
+      <c r="E25" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" s="17">
         <v>14.99</v>
       </c>
-      <c r="I25" s="15">
+      <c r="I25" s="17">
         <v>14.99</v>
       </c>
       <c r="J25" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K25" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="L25" s="19">
+      <c r="K25" s="20">
+        <v>1.0</v>
+      </c>
+      <c r="L25" s="21">
         <f t="shared" si="2"/>
         <v>14.99</v>
       </c>
-      <c r="M25" s="20" t="s">
+      <c r="M25" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="N25" s="20" t="s">
+      <c r="N25" s="22" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2150,45 +2153,45 @@
       <c r="A26" s="4">
         <v>1107.0</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="D26" s="14">
+      <c r="D26" s="16">
         <v>39878.0</v>
       </c>
-      <c r="E26" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F26" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G26" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="H26" s="15">
+      <c r="E26" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H26" s="17">
         <v>14.99</v>
       </c>
-      <c r="I26" s="15">
+      <c r="I26" s="17">
         <v>14.99</v>
       </c>
       <c r="J26" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K26" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="L26" s="19">
+      <c r="K26" s="20">
+        <v>1.0</v>
+      </c>
+      <c r="L26" s="21">
         <f t="shared" si="2"/>
         <v>14.99</v>
       </c>
-      <c r="M26" s="20" t="s">
+      <c r="M26" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="N26" s="20" t="s">
+      <c r="N26" s="22" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2196,45 +2199,45 @@
       <c r="A27" s="4">
         <v>1108.0</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="14">
+      <c r="D27" s="16">
         <v>36266.0</v>
       </c>
-      <c r="E27" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F27" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G27" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="H27" s="15">
+      <c r="E27" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H27" s="17">
         <v>9.99</v>
       </c>
-      <c r="I27" s="15">
+      <c r="I27" s="17">
         <v>9.99</v>
       </c>
       <c r="J27" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K27" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="L27" s="19">
+      <c r="K27" s="20">
+        <v>1.0</v>
+      </c>
+      <c r="L27" s="21">
         <f t="shared" si="2"/>
         <v>9.99</v>
       </c>
-      <c r="M27" s="20" t="s">
+      <c r="M27" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="N27" s="20" t="s">
+      <c r="N27" s="22" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2242,45 +2245,45 @@
       <c r="A28" s="4">
         <v>1109.0</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D28" s="14">
+      <c r="D28" s="16">
         <v>38447.0</v>
       </c>
-      <c r="E28" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F28" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G28" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="H28" s="15">
+      <c r="E28" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H28" s="17">
         <v>14.99</v>
       </c>
-      <c r="I28" s="15">
+      <c r="I28" s="17">
         <v>14.99</v>
       </c>
       <c r="J28" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K28" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="L28" s="19">
+      <c r="K28" s="20">
+        <v>1.0</v>
+      </c>
+      <c r="L28" s="21">
         <f t="shared" si="2"/>
         <v>14.99</v>
       </c>
-      <c r="M28" s="20" t="s">
+      <c r="M28" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="N28" s="20" t="s">
+      <c r="N28" s="22" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2294,7 +2297,7 @@
       <c r="C29" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D29" s="10">
+      <c r="D29" s="11">
         <v>39640.0</v>
       </c>
       <c r="E29" s="4" t="s">
@@ -2306,27 +2309,27 @@
       <c r="G29" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H29" s="11">
+      <c r="H29" s="12">
         <v>9.99</v>
       </c>
-      <c r="I29" s="11">
+      <c r="I29" s="12">
         <v>9.99</v>
       </c>
       <c r="J29" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K29" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="L29" s="19">
+      <c r="K29" s="20">
+        <v>1.0</v>
+      </c>
+      <c r="L29" s="21">
         <f t="shared" si="2"/>
         <v>9.99</v>
       </c>
-      <c r="M29" s="20" t="s">
+      <c r="M29" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="N29" s="20" t="s">
+      <c r="N29" s="22" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2362,17 +2365,17 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K30" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="L30" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M30" s="20" t="s">
+      <c r="K30" s="20">
+        <v>1.0</v>
+      </c>
+      <c r="L30" s="21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M30" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="N30" s="20" t="s">
+      <c r="N30" s="22" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2383,10 +2386,10 @@
       <c r="B31" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="D31" s="14">
+      <c r="D31" s="16">
         <v>45685.0</v>
       </c>
       <c r="E31" s="4" t="s">
@@ -2398,27 +2401,27 @@
       <c r="G31" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H31" s="21">
+      <c r="H31" s="23">
         <v>24.99</v>
       </c>
-      <c r="I31" s="21">
+      <c r="I31" s="23">
         <v>24.99</v>
       </c>
       <c r="J31" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K31" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="L31" s="19">
+      <c r="K31" s="20">
+        <v>1.0</v>
+      </c>
+      <c r="L31" s="21">
         <f t="shared" si="2"/>
         <v>24.99</v>
       </c>
-      <c r="M31" s="20" t="s">
+      <c r="M31" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="N31" s="20" t="s">
+      <c r="N31" s="22" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2432,16 +2435,16 @@
       <c r="C32" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D32" s="12">
+      <c r="D32" s="14">
         <v>45867.0</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F32" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="G32" s="20" t="s">
+      <c r="F32" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32" s="22" t="s">
         <v>18</v>
       </c>
       <c r="H32" s="6">
@@ -2454,17 +2457,17 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K32" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="L32" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M32" s="20" t="s">
+      <c r="K32" s="20">
+        <v>1.0</v>
+      </c>
+      <c r="L32" s="21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M32" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="N32" s="20" t="s">
+      <c r="N32" s="22" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2472,45 +2475,45 @@
       <c r="A33" s="4">
         <v>1114.0</v>
       </c>
-      <c r="B33" s="23" t="s">
+      <c r="B33" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D33" s="14">
+      <c r="D33" s="16">
         <v>45687.0</v>
       </c>
-      <c r="E33" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F33" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G33" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="H33" s="11">
+      <c r="E33" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G33" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H33" s="12">
         <v>17.99</v>
       </c>
-      <c r="I33" s="11">
-        <v>17.99</v>
-      </c>
-      <c r="J33" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K33" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="L33" s="19">
-        <f t="shared" si="2"/>
-        <v>17.99</v>
-      </c>
-      <c r="M33" s="20" t="s">
+      <c r="I33" s="12">
+        <v>12.59</v>
+      </c>
+      <c r="J33" s="13">
+        <f t="shared" si="1"/>
+        <v>5.4</v>
+      </c>
+      <c r="K33" s="20">
+        <v>1.0</v>
+      </c>
+      <c r="L33" s="21">
+        <f t="shared" si="2"/>
+        <v>12.59</v>
+      </c>
+      <c r="M33" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="N33" s="20" t="s">
+      <c r="N33" s="22" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2518,45 +2521,45 @@
       <c r="A34" s="4">
         <v>1115.0</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D34" s="14">
+      <c r="D34" s="16">
         <v>37694.0</v>
       </c>
-      <c r="E34" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F34" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G34" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="H34" s="15">
+      <c r="E34" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G34" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H34" s="17">
         <v>14.99</v>
       </c>
-      <c r="I34" s="15">
+      <c r="I34" s="17">
         <v>14.99</v>
       </c>
       <c r="J34" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K34" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="L34" s="19">
+      <c r="K34" s="20">
+        <v>1.0</v>
+      </c>
+      <c r="L34" s="21">
         <f t="shared" si="2"/>
         <v>14.99</v>
       </c>
-      <c r="M34" s="20" t="s">
+      <c r="M34" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="N34" s="20" t="s">
+      <c r="N34" s="22" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2570,7 +2573,7 @@
       <c r="C35" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D35" s="12">
+      <c r="D35" s="14">
         <v>45785.0</v>
       </c>
       <c r="E35" s="5" t="s">
@@ -2582,27 +2585,27 @@
       <c r="G35" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H35" s="11">
+      <c r="H35" s="12">
         <v>39.99</v>
       </c>
-      <c r="I35" s="11">
-        <v>39.99</v>
-      </c>
-      <c r="J35" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K35" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="L35" s="19">
-        <f t="shared" si="2"/>
-        <v>39.99</v>
-      </c>
-      <c r="M35" s="20" t="s">
+      <c r="I35" s="12">
+        <v>35.99</v>
+      </c>
+      <c r="J35" s="13">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="K35" s="20">
+        <v>1.0</v>
+      </c>
+      <c r="L35" s="21">
+        <f t="shared" si="2"/>
+        <v>35.99</v>
+      </c>
+      <c r="M35" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="N35" s="20" t="s">
+      <c r="N35" s="22" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2638,17 +2641,17 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K36" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="L36" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M36" s="20" t="s">
+      <c r="K36" s="20">
+        <v>1.0</v>
+      </c>
+      <c r="L36" s="21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M36" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="N36" s="20" t="s">
+      <c r="N36" s="22" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2662,16 +2665,16 @@
       <c r="C37" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D37" s="12" t="s">
+      <c r="D37" s="14" t="s">
         <v>16</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F37" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="G37" s="20" t="s">
+      <c r="F37" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G37" s="22" t="s">
         <v>18</v>
       </c>
       <c r="H37" s="6">
@@ -2684,17 +2687,17 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K37" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="L37" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M37" s="20" t="s">
+      <c r="K37" s="20">
+        <v>1.0</v>
+      </c>
+      <c r="L37" s="21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M37" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="N37" s="20" t="s">
+      <c r="N37" s="22" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2702,45 +2705,45 @@
       <c r="A38" s="4">
         <v>1119.0</v>
       </c>
-      <c r="B38" s="25" t="s">
+      <c r="B38" s="28" t="s">
         <v>102</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D38" s="12">
+      <c r="D38" s="14">
         <v>45849.0</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F38" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="G38" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="H38" s="26">
+      <c r="F38" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G38" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H38" s="29">
         <v>25.0</v>
       </c>
-      <c r="I38" s="27">
+      <c r="I38" s="30">
         <v>25.0</v>
       </c>
-      <c r="J38" s="28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K38" s="29">
-        <v>1.0</v>
-      </c>
-      <c r="L38" s="30">
+      <c r="J38" s="31">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K38" s="32">
+        <v>1.0</v>
+      </c>
+      <c r="L38" s="33">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="M38" s="20" t="s">
+      <c r="M38" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="N38" s="20" t="s">
+      <c r="N38" s="22" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2748,45 +2751,45 @@
       <c r="A39" s="4">
         <v>1120.0</v>
       </c>
-      <c r="B39" s="31" t="s">
+      <c r="B39" s="34" t="s">
         <v>104</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D39" s="12">
+      <c r="D39" s="14">
         <v>45849.0</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F39" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="G39" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="H39" s="32">
+      <c r="F39" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G39" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H39" s="35">
         <v>24.99</v>
       </c>
-      <c r="I39" s="33">
+      <c r="I39" s="36">
         <v>24.99</v>
       </c>
-      <c r="J39" s="34">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K39" s="35">
-        <v>1.0</v>
-      </c>
-      <c r="L39" s="36">
+      <c r="J39" s="37">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K39" s="38">
+        <v>1.0</v>
+      </c>
+      <c r="L39" s="39">
         <f t="shared" si="2"/>
         <v>24.99</v>
       </c>
-      <c r="M39" s="20" t="s">
+      <c r="M39" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="N39" s="20" t="s">
+      <c r="N39" s="22" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2800,7 +2803,7 @@
       <c r="C40" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D40" s="10">
+      <c r="D40" s="11">
         <v>45720.0</v>
       </c>
       <c r="E40" s="4" t="s">
@@ -2812,27 +2815,27 @@
       <c r="G40" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H40" s="11">
+      <c r="H40" s="12">
         <v>29.99</v>
       </c>
-      <c r="I40" s="11">
+      <c r="I40" s="12">
         <v>29.99</v>
       </c>
       <c r="J40" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K40" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="L40" s="19">
+      <c r="K40" s="20">
+        <v>1.0</v>
+      </c>
+      <c r="L40" s="21">
         <f t="shared" si="2"/>
         <v>29.99</v>
       </c>
-      <c r="M40" s="20" t="s">
+      <c r="M40" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="N40" s="20" t="s">
+      <c r="N40" s="22" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2846,16 +2849,16 @@
       <c r="C41" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D41" s="12" t="s">
+      <c r="D41" s="14" t="s">
         <v>16</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F41" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G41" s="13" t="s">
+      <c r="F41" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G41" s="15" t="s">
         <v>18</v>
       </c>
       <c r="H41" s="6">
@@ -2868,17 +2871,17 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K41" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="L41" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M41" s="20" t="s">
+      <c r="K41" s="20">
+        <v>1.0</v>
+      </c>
+      <c r="L41" s="21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M41" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="N41" s="20" t="s">
+      <c r="N41" s="22" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2898,10 +2901,10 @@
       <c r="E42" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F42" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G42" s="13" t="s">
+      <c r="F42" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G42" s="15" t="s">
         <v>18</v>
       </c>
       <c r="H42" s="6">
@@ -2914,17 +2917,17 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K42" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="L42" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M42" s="20" t="s">
+      <c r="K42" s="20">
+        <v>1.0</v>
+      </c>
+      <c r="L42" s="21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M42" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="N42" s="20" t="s">
+      <c r="N42" s="22" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2932,45 +2935,45 @@
       <c r="A43" s="4">
         <v>1124.0</v>
       </c>
-      <c r="B43" s="13" t="s">
+      <c r="B43" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="C43" s="13" t="s">
+      <c r="C43" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D43" s="14">
+      <c r="D43" s="16">
         <v>45699.0</v>
       </c>
-      <c r="E43" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F43" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G43" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="H43" s="15">
+      <c r="E43" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F43" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G43" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H43" s="17">
         <v>16.99</v>
       </c>
-      <c r="I43" s="15">
+      <c r="I43" s="17">
         <v>16.99</v>
       </c>
       <c r="J43" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K43" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="L43" s="19">
+      <c r="K43" s="20">
+        <v>1.0</v>
+      </c>
+      <c r="L43" s="21">
         <f t="shared" si="2"/>
         <v>16.99</v>
       </c>
-      <c r="M43" s="20" t="s">
+      <c r="M43" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="N43" s="20" t="s">
+      <c r="N43" s="22" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2984,39 +2987,39 @@
       <c r="C44" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D44" s="10">
+      <c r="D44" s="11">
         <v>45727.0</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F44" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G44" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="H44" s="15">
+      <c r="F44" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G44" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="H44" s="17">
         <v>24.99</v>
       </c>
-      <c r="I44" s="15">
+      <c r="I44" s="17">
         <v>24.99</v>
       </c>
       <c r="J44" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K44" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="L44" s="19">
+      <c r="K44" s="20">
+        <v>1.0</v>
+      </c>
+      <c r="L44" s="21">
         <f t="shared" si="2"/>
         <v>24.99</v>
       </c>
-      <c r="M44" s="20" t="s">
+      <c r="M44" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="N44" s="20" t="s">
+      <c r="N44" s="22" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3036,10 +3039,10 @@
       <c r="E45" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F45" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="G45" s="13" t="s">
+      <c r="F45" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G45" s="15" t="s">
         <v>18</v>
       </c>
       <c r="H45" s="6">
@@ -3052,17 +3055,17 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K45" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="L45" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M45" s="20" t="s">
+      <c r="K45" s="20">
+        <v>1.0</v>
+      </c>
+      <c r="L45" s="21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M45" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="N45" s="20" t="s">
+      <c r="N45" s="22" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3128,10 +3131,10 @@
       <c r="E47" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F47" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="G47" s="20" t="s">
+      <c r="F47" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G47" s="22" t="s">
         <v>18</v>
       </c>
       <c r="H47" s="6">
@@ -3144,17 +3147,17 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K47" s="18">
-        <v>1.0</v>
-      </c>
-      <c r="L47" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M47" s="20" t="s">
+      <c r="K47" s="20">
+        <v>1.0</v>
+      </c>
+      <c r="L47" s="21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M47" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="N47" s="20" t="s">
+      <c r="N47" s="22" t="s">
         <v>122</v>
       </c>
     </row>
@@ -3168,22 +3171,22 @@
       <c r="C48" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D48" s="37" t="s">
+      <c r="D48" s="40" t="s">
         <v>125</v>
       </c>
-      <c r="E48" s="37" t="s">
+      <c r="E48" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="F48" s="37" t="s">
+      <c r="F48" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="G48" s="37" t="s">
+      <c r="G48" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="H48" s="11">
+      <c r="H48" s="12">
         <v>39.99</v>
       </c>
-      <c r="I48" s="11">
+      <c r="I48" s="12">
         <v>39.99</v>
       </c>
       <c r="J48" s="7">
@@ -3208,40 +3211,40 @@
       <c r="A49" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B49" s="38" t="s">
+      <c r="B49" s="4" t="s">
         <v>126</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D49" s="37" t="s">
+      <c r="D49" s="40" t="s">
         <v>125</v>
       </c>
-      <c r="E49" s="37" t="s">
+      <c r="E49" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="F49" s="37" t="s">
+      <c r="F49" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="G49" s="37" t="s">
+      <c r="G49" s="40" t="s">
         <v>123</v>
       </c>
-      <c r="H49" s="11">
+      <c r="H49" s="12">
         <v>39.99</v>
       </c>
-      <c r="I49" s="11">
-        <v>19.99</v>
-      </c>
-      <c r="J49" s="39">
-        <f t="shared" si="1"/>
-        <v>20</v>
+      <c r="I49" s="12">
+        <v>39.99</v>
+      </c>
+      <c r="J49" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="K49" s="8">
         <v>1.0</v>
       </c>
       <c r="L49" s="9">
         <f t="shared" si="2"/>
-        <v>19.99</v>
+        <v>39.99</v>
       </c>
       <c r="M49" s="4" t="s">
         <v>123</v>
@@ -3252,47 +3255,47 @@
     </row>
     <row r="50">
       <c r="A50" s="4"/>
-      <c r="B50" s="40"/>
+      <c r="B50" s="41"/>
       <c r="C50" s="8"/>
-      <c r="D50" s="40"/>
-      <c r="E50" s="41"/>
-      <c r="F50" s="41"/>
-      <c r="G50" s="42">
+      <c r="D50" s="41"/>
+      <c r="E50" s="42"/>
+      <c r="F50" s="42"/>
+      <c r="G50" s="43">
         <f>COUNTA(A2:A49)</f>
         <v>48</v>
       </c>
-      <c r="H50" s="43">
+      <c r="H50" s="44">
         <f t="shared" ref="H50:I50" si="3">SUM(H2:H49)</f>
-        <v>639.73</v>
-      </c>
-      <c r="I50" s="43">
+        <v>649.73</v>
+      </c>
+      <c r="I50" s="44">
         <f t="shared" si="3"/>
-        <v>619.73</v>
-      </c>
-      <c r="J50" s="43">
-        <f t="shared" si="1"/>
-        <v>20</v>
-      </c>
-      <c r="K50" s="41"/>
-      <c r="L50" s="41"/>
-      <c r="M50" s="41"/>
-      <c r="N50" s="41"/>
+        <v>617.98</v>
+      </c>
+      <c r="J50" s="44">
+        <f t="shared" si="1"/>
+        <v>31.75</v>
+      </c>
+      <c r="K50" s="42"/>
+      <c r="L50" s="42"/>
+      <c r="M50" s="42"/>
+      <c r="N50" s="42"/>
     </row>
     <row r="51">
       <c r="A51" s="4"/>
-      <c r="B51" s="40"/>
+      <c r="B51" s="41"/>
       <c r="C51" s="8"/>
-      <c r="D51" s="41"/>
-      <c r="E51" s="41"/>
-      <c r="F51" s="41"/>
-      <c r="G51" s="41"/>
-      <c r="H51" s="41"/>
-      <c r="I51" s="41"/>
-      <c r="J51" s="41"/>
-      <c r="K51" s="41"/>
-      <c r="L51" s="41"/>
-      <c r="M51" s="41"/>
-      <c r="N51" s="41"/>
+      <c r="D51" s="42"/>
+      <c r="E51" s="42"/>
+      <c r="F51" s="42"/>
+      <c r="G51" s="42"/>
+      <c r="H51" s="42"/>
+      <c r="I51" s="42"/>
+      <c r="J51" s="42"/>
+      <c r="K51" s="42"/>
+      <c r="L51" s="42"/>
+      <c r="M51" s="42"/>
+      <c r="N51" s="42"/>
     </row>
     <row r="52">
       <c r="A52" s="1" t="s">
@@ -3339,108 +3342,108 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="44">
+      <c r="A53" s="45">
         <v>1082.0</v>
       </c>
-      <c r="B53" s="44" t="s">
+      <c r="B53" s="45" t="s">
         <v>127</v>
       </c>
-      <c r="C53" s="44" t="s">
+      <c r="C53" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="D53" s="45">
+      <c r="D53" s="46">
         <v>45078.0</v>
       </c>
-      <c r="E53" s="45">
+      <c r="E53" s="46">
         <v>45734.0</v>
       </c>
-      <c r="F53" s="45">
+      <c r="F53" s="46">
         <v>45734.0</v>
       </c>
-      <c r="G53" s="45">
+      <c r="G53" s="46">
         <v>45734.0</v>
       </c>
-      <c r="H53" s="46">
+      <c r="H53" s="47">
         <v>24.99</v>
       </c>
-      <c r="I53" s="46">
+      <c r="I53" s="47">
         <v>8.49</v>
       </c>
-      <c r="J53" s="39">
+      <c r="J53" s="13">
         <f>H53-I53</f>
         <v>16.5</v>
       </c>
-      <c r="K53" s="47">
-        <v>1.0</v>
-      </c>
-      <c r="L53" s="48">
+      <c r="K53" s="48">
+        <v>1.0</v>
+      </c>
+      <c r="L53" s="49">
         <f>I53/K53</f>
         <v>8.49</v>
       </c>
-      <c r="M53" s="44" t="s">
+      <c r="M53" s="45" t="s">
         <v>128</v>
       </c>
-      <c r="N53" s="44" t="s">
+      <c r="N53" s="45" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="24"/>
-      <c r="B54" s="40"/>
+      <c r="A54" s="26"/>
+      <c r="B54" s="41"/>
       <c r="C54" s="8"/>
-      <c r="D54" s="49"/>
-      <c r="E54" s="41"/>
-      <c r="F54" s="41"/>
-      <c r="G54" s="41"/>
-      <c r="H54" s="50"/>
-      <c r="I54" s="50"/>
-      <c r="J54" s="50"/>
-      <c r="K54" s="41"/>
-      <c r="L54" s="50"/>
-      <c r="M54" s="41"/>
-      <c r="N54" s="41"/>
+      <c r="D54" s="50"/>
+      <c r="E54" s="42"/>
+      <c r="F54" s="42"/>
+      <c r="G54" s="42"/>
+      <c r="H54" s="51"/>
+      <c r="I54" s="51"/>
+      <c r="J54" s="51"/>
+      <c r="K54" s="42"/>
+      <c r="L54" s="51"/>
+      <c r="M54" s="42"/>
+      <c r="N54" s="42"/>
     </row>
     <row r="55">
-      <c r="A55" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="B55" s="52" t="s">
+      <c r="A55" s="52" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="C55" s="52" t="s">
+      <c r="C55" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="D55" s="52" t="s">
+      <c r="D55" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="E55" s="52" t="s">
+      <c r="E55" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="F55" s="52" t="s">
+      <c r="F55" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="G55" s="52" t="s">
+      <c r="G55" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="H55" s="52" t="s">
+      <c r="H55" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="I55" s="53" t="s">
+      <c r="I55" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="J55" s="52" t="s">
+      <c r="J55" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="K55" s="52" t="s">
+      <c r="K55" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="L55" s="52" t="s">
+      <c r="L55" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="M55" s="52" t="s">
+      <c r="M55" s="53" t="s">
         <v>12</v>
       </c>
-      <c r="N55" s="52" t="s">
+      <c r="N55" s="53" t="s">
         <v>13</v>
       </c>
     </row>
@@ -3452,7 +3455,7 @@
       <c r="C56" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D56" s="41"/>
+      <c r="D56" s="42"/>
       <c r="E56" s="4" t="s">
         <v>17</v>
       </c>
@@ -3462,10 +3465,10 @@
       <c r="G56" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H56" s="11">
+      <c r="H56" s="12">
         <v>59.99</v>
       </c>
-      <c r="I56" s="11">
+      <c r="I56" s="12">
         <v>59.99</v>
       </c>
       <c r="J56" s="9">
@@ -3494,7 +3497,7 @@
       <c r="C57" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D57" s="40"/>
+      <c r="D57" s="41"/>
       <c r="E57" s="4" t="s">
         <v>17</v>
       </c>
@@ -3504,10 +3507,10 @@
       <c r="G57" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H57" s="11">
+      <c r="H57" s="12">
         <v>34.99</v>
       </c>
-      <c r="I57" s="11">
+      <c r="I57" s="12">
         <v>34.99</v>
       </c>
       <c r="J57" s="9">
@@ -3536,7 +3539,7 @@
       <c r="C58" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D58" s="40"/>
+      <c r="D58" s="41"/>
       <c r="E58" s="4" t="s">
         <v>17</v>
       </c>
@@ -3546,10 +3549,10 @@
       <c r="G58" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H58" s="11">
+      <c r="H58" s="12">
         <v>49.99</v>
       </c>
-      <c r="I58" s="11">
+      <c r="I58" s="12">
         <v>49.99</v>
       </c>
       <c r="J58" s="9">
@@ -3578,7 +3581,7 @@
       <c r="C59" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D59" s="40"/>
+      <c r="D59" s="41"/>
       <c r="E59" s="4" t="s">
         <v>17</v>
       </c>
@@ -3588,10 +3591,10 @@
       <c r="G59" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H59" s="11">
+      <c r="H59" s="12">
         <v>49.99</v>
       </c>
-      <c r="I59" s="11">
+      <c r="I59" s="12">
         <v>49.99</v>
       </c>
       <c r="J59" s="9">
@@ -3620,7 +3623,7 @@
       <c r="C60" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D60" s="41"/>
+      <c r="D60" s="42"/>
       <c r="E60" s="4" t="s">
         <v>17</v>
       </c>
@@ -3630,10 +3633,10 @@
       <c r="G60" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H60" s="11">
+      <c r="H60" s="12">
         <v>54.99</v>
       </c>
-      <c r="I60" s="11">
+      <c r="I60" s="12">
         <v>54.99</v>
       </c>
       <c r="J60" s="9">

</xml_diff>